<commit_message>
correcting percent change data
</commit_message>
<xml_diff>
--- a/data/historical prices/aapl2.xlsx
+++ b/data/historical prices/aapl2.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="-34120" yWindow="2380" windowWidth="28800" windowHeight="16280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="aapl2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -363,7 +363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I548"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A539" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A537" workbookViewId="0">
       <selection activeCell="C505" sqref="C505"/>
     </sheetView>
   </sheetViews>
@@ -7802,8 +7802,8 @@
         <v>104.48</v>
       </c>
       <c r="C369" s="2">
-        <f>B369/B368-1</f>
-        <v>-1.4804337576614701E-2</v>
+        <f>B369/B365-1</f>
+        <v>1.4861583292860692E-2</v>
       </c>
       <c r="D369">
         <v>106.05</v>

</xml_diff>